<commit_message>
-Moved writeback MUX to MEM1 -Fixed enable for ports
</commit_message>
<xml_diff>
--- a/Instruction bit details.xlsx
+++ b/Instruction bit details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h4z3m\Desktop\Files\College\3rd\2nd Semester\CMPN301\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5166799-6ED9-474F-97D2-0DD510EDB30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84362E24-5512-4404-8B36-59FD143EC745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{6DA1F6BA-0999-4314-B85B-1DD813E74D7B}"/>
+    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11100" activeTab="1" xr2:uid="{6DA1F6BA-0999-4314-B85B-1DD813E74D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2242,10 +2242,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}" name="Table1" displayName="Table1" ref="B1:S28" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B1:S28" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}"/>
@@ -2605,8 +2601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FB175E-1B2E-49A1-9201-CF52D899FEF0}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:XFD8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,7 +2614,8 @@
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="11" width="15" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="22" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
   </cols>
@@ -4280,8 +4277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE8E6B-46C5-4A7D-9C9D-87C2DC308357}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5869,6 +5866,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100642169E4106A8F47AE930E47A554F108" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d50252937a7f2e196425f0325211b942">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edbcc27db5b7c97cc0de701a4705ae6f">
     <xsd:element name="properties">
@@ -5982,15 +5988,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C9F5D58-F0B6-4055-A760-0A329106689F}">
   <ds:schemaRefs>
@@ -6007,6 +6004,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3469B4E-C240-470A-B28C-1875F0C71483}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF32969-1B70-433C-9090-E0745F49E89E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6020,12 +6025,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3469B4E-C240-470A-B28C-1875F0C71483}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
-Added MUX's before and after PC
</commit_message>
<xml_diff>
--- a/Instruction bit details.xlsx
+++ b/Instruction bit details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h4z3m\Desktop\Files\College\3rd\2nd Semester\CMPN301\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84362E24-5512-4404-8B36-59FD143EC745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06AE490-0F6C-4FBD-B4CB-62F748D97F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="18900" windowHeight="11100" activeTab="1" xr2:uid="{6DA1F6BA-0999-4314-B85B-1DD813E74D7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="1" xr2:uid="{6DA1F6BA-0999-4314-B85B-1DD813E74D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="107">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -198,9 +198,6 @@
     <t>ADD</t>
   </si>
   <si>
-    <t>011 xxx</t>
-  </si>
-  <si>
     <t>Flag</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>MOV</t>
   </si>
   <si>
-    <t>010 xxx</t>
-  </si>
-  <si>
     <t>NOT</t>
   </si>
   <si>
@@ -339,13 +333,31 @@
     <t>000 110</t>
   </si>
   <si>
-    <t>100 xxx</t>
-  </si>
-  <si>
-    <t>101 xxx</t>
-  </si>
-  <si>
     <t>101 000</t>
+  </si>
+  <si>
+    <t>011 100</t>
+  </si>
+  <si>
+    <t>011 001</t>
+  </si>
+  <si>
+    <t>011 110</t>
+  </si>
+  <si>
+    <t>011 111</t>
+  </si>
+  <si>
+    <t>010 000</t>
+  </si>
+  <si>
+    <t>011 011</t>
+  </si>
+  <si>
+    <t>011 010</t>
+  </si>
+  <si>
+    <t>011 101</t>
   </si>
 </sst>
 </file>
@@ -426,7 +438,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +466,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -816,11 +834,21 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2243,60 +2271,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}" name="Table1" displayName="Table1" ref="B1:S28" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}" name="Table1" displayName="Table1" ref="B1:S28" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <autoFilter ref="B1:S28" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:S27">
-    <sortCondition sortBy="fontColor" ref="B1:B27" dxfId="42"/>
-  </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{8D4E3407-FC44-47DE-B88E-5309AD11F2D5}" name="Instruction" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{25C21E2B-6DEE-4078-B4A9-EA2552352DD6}" name="Mem-read" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{C5397294-29B8-4F09-9F40-E9166D94F2FE}" name="Mem-write" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{FECC954A-7C1B-40D2-86A2-FD9B4A391E20}" name="ALU src" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{23D8C483-4386-4311-BB2B-EEE7E1B86230}" name="ALU op" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{06ADF1F3-3ED4-4830-AEBB-7387DC1D335D}" name="Mem-to-reg" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{6D259160-FBA0-4881-8B80-2A2B2619FD03}" name="Branch" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{0FB6092E-1557-4466-BD9B-B56A99A8E22D}" name="Jump" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{35C25808-AE3A-4B3F-99C7-79DDCCDF49D7}" name="RegDst" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{854CF863-3B0A-454A-8E03-87707C60D946}" name="RegWrite" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{D335D4AE-F1D6-4066-A7B1-CBD1203DC43A}" name="Port EN" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{C2F17218-CFFA-4D13-AE38-39C5A8EF6E7F}" name="FlagEN" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{D4D559F1-71F0-460D-BBFF-425684E0F856}" name="Column2" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{8F9EB460-835A-4CD7-AE5D-948217152F0C}" name="OpCode[5:4]" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{CE15952D-D927-4D54-BC82-6955E131E454}" name="OpCode[3]" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{9CF82271-0E8F-4CD8-9691-5677AACE840C}" name="OpCode[2]" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{A5F2F74E-484F-4C42-83E9-34E52A647D2E}" name="OpCode[1]" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{44C370CE-309A-4F3E-9449-2EC3F32FA845}" name="OpCode[0]" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{8D4E3407-FC44-47DE-B88E-5309AD11F2D5}" name="Instruction" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{25C21E2B-6DEE-4078-B4A9-EA2552352DD6}" name="Mem-read" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{C5397294-29B8-4F09-9F40-E9166D94F2FE}" name="Mem-write" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{FECC954A-7C1B-40D2-86A2-FD9B4A391E20}" name="ALU src" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{23D8C483-4386-4311-BB2B-EEE7E1B86230}" name="ALU op" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{06ADF1F3-3ED4-4830-AEBB-7387DC1D335D}" name="Mem-to-reg" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{6D259160-FBA0-4881-8B80-2A2B2619FD03}" name="Branch" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{0FB6092E-1557-4466-BD9B-B56A99A8E22D}" name="Jump" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{35C25808-AE3A-4B3F-99C7-79DDCCDF49D7}" name="RegDst" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{854CF863-3B0A-454A-8E03-87707C60D946}" name="RegWrite" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{D335D4AE-F1D6-4066-A7B1-CBD1203DC43A}" name="Port EN" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{C2F17218-CFFA-4D13-AE38-39C5A8EF6E7F}" name="FlagEN" dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{D4D559F1-71F0-460D-BBFF-425684E0F856}" name="Column2" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{8F9EB460-835A-4CD7-AE5D-948217152F0C}" name="OpCode[5:4]" dataDxfId="29"/>
+    <tableColumn id="15" xr3:uid="{CE15952D-D927-4D54-BC82-6955E131E454}" name="OpCode[3]" dataDxfId="28"/>
+    <tableColumn id="16" xr3:uid="{9CF82271-0E8F-4CD8-9691-5677AACE840C}" name="OpCode[2]" dataDxfId="27"/>
+    <tableColumn id="17" xr3:uid="{A5F2F74E-484F-4C42-83E9-34E52A647D2E}" name="OpCode[1]" dataDxfId="26"/>
+    <tableColumn id="18" xr3:uid="{44C370CE-309A-4F3E-9449-2EC3F32FA845}" name="OpCode[0]" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{37C617F5-F877-4DEE-8F3D-693EC682D08C}" name="Table13" displayName="Table13" ref="A1:R28" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{37C617F5-F877-4DEE-8F3D-693EC682D08C}" name="Table13" displayName="Table13" ref="A1:R28" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A1:R28" xr:uid="{37C617F5-F877-4DEE-8F3D-693EC682D08C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R7">
     <sortCondition descending="1" ref="K1:K28"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{E706B79B-C3DE-40F8-8984-F90F324F38F1}" name="Instruction" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{E468DF59-6FA2-454C-A7C9-03CF45E90DFB}" name="Mem-read" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{F0E5CDCB-CD17-4F6F-99AE-47C914BBD130}" name="Mem-write" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{EAFC9A0C-24CC-4EB3-BAC2-0902DD99D451}" name="ALU src" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{72E04338-F7FE-487C-9B7C-A26811E62A38}" name="ALU op" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{A5657D19-E2E9-4349-B830-DEE87B2354AC}" name="Mem-to-reg" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{81E8A75B-C17A-4132-9D7E-2E6D2FFC70FA}" name="Branch" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{606669A1-E1A7-477E-9923-6F2C21718722}" name="Jump" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{0F6141CD-6F16-41E1-B2C7-0E368AA607E1}" name="RegDst" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{7CB9D208-D2DE-4200-8FF1-505E1FB4C112}" name="RegWrite" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{8DDC56CF-0E9C-4CE6-A782-0A8FC6FFFE69}" name="Port EN" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{4E4D1F5E-7525-4563-A551-437CC225A0A6}" name="FlagEN" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{D63ABDED-CA31-4388-8E46-DB793355A769}" name="Column2" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{7F48F358-6CED-4C7E-8A8E-28F0B0755D7F}" name="Column3" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{1DEF6221-63F2-447A-8A17-553930013B73}" name="Column4" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{A1FBB6C0-AE90-4897-B30C-3FB013B898E2}" name="Column5" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{218E459E-5EAC-478C-997C-AEC3C336D5A5}" name="Column6" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{4FC20EE3-62CA-4D56-BB07-A9DF668D2B4A}" name="Column7" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E706B79B-C3DE-40F8-8984-F90F324F38F1}" name="Instruction" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{E468DF59-6FA2-454C-A7C9-03CF45E90DFB}" name="Mem-read" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{F0E5CDCB-CD17-4F6F-99AE-47C914BBD130}" name="Mem-write" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{EAFC9A0C-24CC-4EB3-BAC2-0902DD99D451}" name="ALU src" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{72E04338-F7FE-487C-9B7C-A26811E62A38}" name="ALU op" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{A5657D19-E2E9-4349-B830-DEE87B2354AC}" name="Mem-to-reg" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{81E8A75B-C17A-4132-9D7E-2E6D2FFC70FA}" name="Branch" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{606669A1-E1A7-477E-9923-6F2C21718722}" name="Jump" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{0F6141CD-6F16-41E1-B2C7-0E368AA607E1}" name="RegDst" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{7CB9D208-D2DE-4200-8FF1-505E1FB4C112}" name="RegWrite" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{8DDC56CF-0E9C-4CE6-A782-0A8FC6FFFE69}" name="Port EN" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{4E4D1F5E-7525-4563-A551-437CC225A0A6}" name="FlagEN" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{D63ABDED-CA31-4388-8E46-DB793355A769}" name="Column2" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{7F48F358-6CED-4C7E-8A8E-28F0B0755D7F}" name="Column3" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{1DEF6221-63F2-447A-8A17-553930013B73}" name="Column4" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{A1FBB6C0-AE90-4897-B30C-3FB013B898E2}" name="Column5" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{218E459E-5EAC-478C-997C-AEC3C336D5A5}" name="Column6" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{4FC20EE3-62CA-4D56-BB07-A9DF668D2B4A}" name="Column7" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2601,26 +2626,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FB175E-1B2E-49A1-9201-CF52D899FEF0}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24:I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="22" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2679,7 +2708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2738,7 +2767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
         <v>25</v>
       </c>
@@ -2794,7 +2823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="29" t="s">
         <v>30</v>
       </c>
@@ -2850,7 +2879,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="29" t="s">
         <v>32</v>
       </c>
@@ -2906,7 +2935,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="29" t="s">
         <v>35</v>
       </c>
@@ -2962,7 +2991,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="26" t="s">
         <v>37</v>
       </c>
@@ -3018,7 +3047,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="26" t="s">
         <v>42</v>
       </c>
@@ -3074,7 +3103,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="26" t="s">
         <v>45</v>
       </c>
@@ -3130,7 +3159,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="26" t="s">
         <v>47</v>
       </c>
@@ -3186,7 +3215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="26" t="s">
         <v>49</v>
       </c>
@@ -3242,7 +3271,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -3282,29 +3311,29 @@
       <c r="M12" s="25">
         <v>1</v>
       </c>
-      <c r="N12" s="21" t="s">
-        <v>53</v>
+      <c r="N12" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="O12" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>1</v>
+      </c>
+      <c r="R12" s="10">
+        <v>0</v>
+      </c>
+      <c r="S12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="Q12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S12" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
-        <v>55</v>
-      </c>
       <c r="C13" s="24">
         <v>0</v>
       </c>
@@ -3338,28 +3367,28 @@
       <c r="M13" s="25">
         <v>1</v>
       </c>
-      <c r="N13" s="21" t="s">
-        <v>53</v>
+      <c r="N13" s="43" t="s">
+        <v>100</v>
       </c>
       <c r="O13" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S13" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0</v>
+      </c>
+      <c r="S13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="24">
         <v>0</v>
@@ -3394,28 +3423,28 @@
       <c r="M14" s="25">
         <v>1</v>
       </c>
-      <c r="N14" s="21" t="s">
-        <v>53</v>
+      <c r="N14" s="43" t="s">
+        <v>101</v>
       </c>
       <c r="O14" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S14" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>1</v>
+      </c>
+      <c r="R14" s="10">
+        <v>1</v>
+      </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="24">
         <v>0</v>
@@ -3450,28 +3479,28 @@
       <c r="M15" s="25">
         <v>1</v>
       </c>
-      <c r="N15" s="21" t="s">
-        <v>53</v>
+      <c r="N15" s="43" t="s">
+        <v>102</v>
       </c>
       <c r="O15" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S15" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>1</v>
+      </c>
+      <c r="R15" s="10">
+        <v>1</v>
+      </c>
+      <c r="S15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="24">
         <v>0</v>
@@ -3506,28 +3535,28 @@
       <c r="M16" s="25">
         <v>0</v>
       </c>
-      <c r="N16" s="21" t="s">
-        <v>59</v>
+      <c r="N16" s="43" t="s">
+        <v>103</v>
       </c>
       <c r="O16" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S16" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>0</v>
+      </c>
+      <c r="R16" s="10">
+        <v>0</v>
+      </c>
+      <c r="S16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="24">
         <v>0</v>
@@ -3562,28 +3591,28 @@
       <c r="M17" s="25">
         <v>1</v>
       </c>
-      <c r="N17" s="21" t="s">
-        <v>53</v>
+      <c r="N17" s="43" t="s">
+        <v>104</v>
       </c>
       <c r="O17" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S17" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>0</v>
+      </c>
+      <c r="R17" s="10">
+        <v>1</v>
+      </c>
+      <c r="S17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="24">
         <v>0</v>
@@ -3618,28 +3647,28 @@
       <c r="M18" s="25">
         <v>1</v>
       </c>
-      <c r="N18" s="21" t="s">
-        <v>53</v>
+      <c r="N18" s="43" t="s">
+        <v>105</v>
       </c>
       <c r="O18" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S18" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>0</v>
+      </c>
+      <c r="R18" s="10">
+        <v>1</v>
+      </c>
+      <c r="S18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" s="24">
         <v>0</v>
@@ -3674,28 +3703,28 @@
       <c r="M19" s="25">
         <v>1</v>
       </c>
-      <c r="N19" s="21" t="s">
-        <v>53</v>
+      <c r="N19" s="43" t="s">
+        <v>106</v>
       </c>
       <c r="O19" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S19" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>1</v>
+      </c>
+      <c r="R19" s="10">
+        <v>0</v>
+      </c>
+      <c r="S19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -3731,7 +3760,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O20" s="32" t="s">
         <v>22</v>
@@ -3749,9 +3778,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" s="16">
         <v>0</v>
@@ -3787,16 +3816,16 @@
         <v>1</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O21" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q21" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R21" s="10" t="s">
         <v>23</v>
@@ -3805,48 +3834,48 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="G22" s="13">
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
+        <v>1</v>
+      </c>
+      <c r="I22" s="13">
+        <v>0</v>
+      </c>
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
+        <v>0</v>
+      </c>
+      <c r="M22" s="14">
+        <v>0</v>
+      </c>
+      <c r="N22" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" s="13">
-        <v>0</v>
-      </c>
-      <c r="D22" s="13">
-        <v>0</v>
-      </c>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0</v>
-      </c>
-      <c r="H22" s="13">
-        <v>1</v>
-      </c>
-      <c r="I22" s="13">
-        <v>0</v>
-      </c>
-      <c r="J22" s="13">
-        <v>0</v>
-      </c>
-      <c r="K22" s="13">
-        <v>0</v>
-      </c>
-      <c r="L22" s="13">
-        <v>0</v>
-      </c>
-      <c r="M22" s="14">
-        <v>0</v>
-      </c>
-      <c r="N22" s="21" t="s">
-        <v>72</v>
       </c>
       <c r="O22" s="32" t="s">
         <v>22</v>
@@ -3855,7 +3884,7 @@
         <v>8</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R22" s="10" t="s">
         <v>41</v>
@@ -3864,45 +3893,45 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="13">
+        <v>0</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
+      <c r="I23" s="13">
+        <v>0</v>
+      </c>
+      <c r="J23" s="13">
+        <v>0</v>
+      </c>
+      <c r="K23" s="13">
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
+        <v>0</v>
+      </c>
+      <c r="M23" s="14">
+        <v>0</v>
+      </c>
+      <c r="N23" s="21" t="s">
         <v>74</v>
-      </c>
-      <c r="C23" s="13">
-        <v>0</v>
-      </c>
-      <c r="D23" s="13">
-        <v>0</v>
-      </c>
-      <c r="E23" s="13">
-        <v>0</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="13">
-        <v>0</v>
-      </c>
-      <c r="H23" s="13">
-        <v>1</v>
-      </c>
-      <c r="I23" s="13">
-        <v>0</v>
-      </c>
-      <c r="J23" s="13">
-        <v>0</v>
-      </c>
-      <c r="K23" s="13">
-        <v>0</v>
-      </c>
-      <c r="L23" s="13">
-        <v>0</v>
-      </c>
-      <c r="M23" s="14">
-        <v>0</v>
-      </c>
-      <c r="N23" s="21" t="s">
-        <v>76</v>
       </c>
       <c r="O23" s="32" t="s">
         <v>22</v>
@@ -3911,7 +3940,7 @@
         <v>8</v>
       </c>
       <c r="Q23" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="R23" s="10" t="s">
         <v>41</v>
@@ -3920,9 +3949,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C24" s="16">
         <v>0</v>
@@ -3958,16 +3987,16 @@
         <v>0</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O24" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R24" s="10" t="s">
         <v>23</v>
@@ -3976,9 +4005,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="16">
         <v>0</v>
@@ -4014,16 +4043,16 @@
         <v>0</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O25" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P25" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q25" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R25" s="10" t="s">
         <v>23</v>
@@ -4032,9 +4061,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" s="16">
         <v>1</v>
@@ -4070,16 +4099,16 @@
         <v>0</v>
       </c>
       <c r="N26" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O26" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R26" s="10" t="s">
         <v>23</v>
@@ -4088,9 +4117,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="38">
         <v>1</v>
@@ -4126,16 +4155,16 @@
         <v>1</v>
       </c>
       <c r="N27" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O27" s="32" t="s">
         <v>22</v>
       </c>
       <c r="P27" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q27" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R27" s="10" t="s">
         <v>23</v>
@@ -4144,7 +4173,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B28" s="40"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -4159,7 +4188,7 @@
       <c r="M28" s="9"/>
       <c r="N28" s="41"/>
       <c r="O28" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P28" s="8">
         <v>29</v>
@@ -4174,61 +4203,61 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>87</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
         <v>88</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>90</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -4237,7 +4266,7 @@
         <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F55" t="s">
         <v>41</v>
@@ -4246,9 +4275,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4263,7 +4292,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="N2:N28">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4277,13 +4306,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE8E6B-46C5-4A7D-9C9D-87C2DC308357}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -4324,24 +4356,24 @@
         <v>13</v>
       </c>
       <c r="N1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
-        <v>98</v>
       </c>
       <c r="B2" s="24">
         <v>0</v>
@@ -4377,7 +4409,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N2" s="33" t="s">
         <v>22</v>
@@ -4395,7 +4427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
         <v>32</v>
       </c>
@@ -4451,7 +4483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
         <v>25</v>
       </c>
@@ -4507,7 +4539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>20</v>
       </c>
@@ -4563,7 +4595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>30</v>
       </c>
@@ -4619,7 +4651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
         <v>35</v>
       </c>
@@ -4675,7 +4707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>42</v>
       </c>
@@ -4731,7 +4763,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>47</v>
       </c>
@@ -4787,7 +4819,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>37</v>
       </c>
@@ -4843,7 +4875,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>45</v>
       </c>
@@ -4899,7 +4931,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>49</v>
       </c>
@@ -4955,9 +4987,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="24">
         <v>0</v>
@@ -4992,28 +5024,28 @@
       <c r="L13" s="25">
         <v>1</v>
       </c>
-      <c r="M13" s="21" t="s">
-        <v>100</v>
+      <c r="M13" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="N13" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R13" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="P13" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="24">
         <v>0</v>
@@ -5048,28 +5080,28 @@
       <c r="L14" s="25">
         <v>1</v>
       </c>
-      <c r="M14" s="21" t="s">
-        <v>101</v>
+      <c r="M14" s="43" t="s">
+        <v>100</v>
       </c>
       <c r="N14" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>0</v>
+      </c>
+      <c r="R14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="24">
         <v>0</v>
@@ -5104,26 +5136,26 @@
       <c r="L15" s="25">
         <v>1</v>
       </c>
-      <c r="M15" s="21" t="s">
+      <c r="M15" s="43" t="s">
         <v>101</v>
       </c>
       <c r="N15" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="P15" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>1</v>
+      </c>
+      <c r="R15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
         <v>52</v>
       </c>
@@ -5160,28 +5192,28 @@
       <c r="L16" s="25">
         <v>1</v>
       </c>
-      <c r="M16" s="21" t="s">
-        <v>101</v>
+      <c r="M16" s="43" t="s">
+        <v>102</v>
       </c>
       <c r="N16" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="P16" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>1</v>
+      </c>
+      <c r="R16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="24">
         <v>0</v>
@@ -5216,29 +5248,29 @@
       <c r="L17" s="25">
         <v>1</v>
       </c>
-      <c r="M17" s="21" t="s">
-        <v>101</v>
+      <c r="M17" s="43" t="s">
+        <v>103</v>
       </c>
       <c r="N17" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="P17" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>0</v>
+      </c>
+      <c r="R17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="P17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R17" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
-        <v>55</v>
-      </c>
       <c r="B18" s="24">
         <v>0</v>
       </c>
@@ -5272,28 +5304,28 @@
       <c r="L18" s="25">
         <v>1</v>
       </c>
-      <c r="M18" s="21" t="s">
-        <v>101</v>
+      <c r="M18" s="43" t="s">
+        <v>104</v>
       </c>
       <c r="N18" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="P18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>1</v>
+      </c>
+      <c r="R18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B19" s="24">
         <v>0</v>
@@ -5328,28 +5360,28 @@
       <c r="L19" s="25">
         <v>1</v>
       </c>
-      <c r="M19" s="21" t="s">
-        <v>101</v>
+      <c r="M19" s="43" t="s">
+        <v>105</v>
       </c>
       <c r="N19" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R19" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="P19" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>1</v>
+      </c>
+      <c r="R19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="24">
         <v>0</v>
@@ -5384,64 +5416,64 @@
       <c r="L20" s="25">
         <v>0</v>
       </c>
-      <c r="M20" s="21" t="s">
-        <v>100</v>
+      <c r="M20" s="43" t="s">
+        <v>106</v>
       </c>
       <c r="N20" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="P20" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q20" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="P20" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>0</v>
+      </c>
+      <c r="R20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0</v>
+      </c>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <v>0</v>
+      </c>
+      <c r="L21" s="14">
+        <v>0</v>
+      </c>
+      <c r="M21" s="21" t="s">
         <v>74</v>
-      </c>
-      <c r="B21" s="13">
-        <v>0</v>
-      </c>
-      <c r="C21" s="13">
-        <v>0</v>
-      </c>
-      <c r="D21" s="13">
-        <v>0</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="13">
-        <v>0</v>
-      </c>
-      <c r="G21" s="13">
-        <v>1</v>
-      </c>
-      <c r="H21" s="13">
-        <v>0</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0</v>
-      </c>
-      <c r="J21" s="13">
-        <v>0</v>
-      </c>
-      <c r="K21" s="13">
-        <v>0</v>
-      </c>
-      <c r="L21" s="14">
-        <v>0</v>
-      </c>
-      <c r="M21" s="21" t="s">
-        <v>76</v>
       </c>
       <c r="N21" s="32" t="s">
         <v>22</v>
@@ -5450,7 +5482,7 @@
         <v>8</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q21" s="10" t="s">
         <v>41</v>
@@ -5459,45 +5491,45 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13">
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
+        <v>0</v>
+      </c>
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0</v>
+      </c>
+      <c r="L22" s="14">
+        <v>0</v>
+      </c>
+      <c r="M22" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="B22" s="13">
-        <v>0</v>
-      </c>
-      <c r="C22" s="13">
-        <v>0</v>
-      </c>
-      <c r="D22" s="13">
-        <v>0</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="13">
-        <v>0</v>
-      </c>
-      <c r="G22" s="13">
-        <v>1</v>
-      </c>
-      <c r="H22" s="13">
-        <v>0</v>
-      </c>
-      <c r="I22" s="13">
-        <v>0</v>
-      </c>
-      <c r="J22" s="13">
-        <v>0</v>
-      </c>
-      <c r="K22" s="13">
-        <v>0</v>
-      </c>
-      <c r="L22" s="14">
-        <v>0</v>
-      </c>
-      <c r="M22" s="21" t="s">
-        <v>72</v>
       </c>
       <c r="N22" s="32" t="s">
         <v>22</v>
@@ -5506,7 +5538,7 @@
         <v>8</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q22" s="10" t="s">
         <v>41</v>
@@ -5515,9 +5547,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" s="16">
         <v>0</v>
@@ -5553,16 +5585,16 @@
         <v>0</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N23" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P23" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q23" s="10" t="s">
         <v>23</v>
@@ -5571,9 +5603,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="16">
         <v>0</v>
@@ -5609,16 +5641,16 @@
         <v>0</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N24" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q24" s="10" t="s">
         <v>23</v>
@@ -5627,9 +5659,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" s="16">
         <v>1</v>
@@ -5665,16 +5697,16 @@
         <v>0</v>
       </c>
       <c r="M25" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N25" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P25" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q25" s="10" t="s">
         <v>23</v>
@@ -5683,9 +5715,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" s="16">
         <v>1</v>
@@ -5721,16 +5753,16 @@
         <v>1</v>
       </c>
       <c r="M26" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N26" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>23</v>
@@ -5739,9 +5771,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="16">
         <v>0</v>
@@ -5777,16 +5809,16 @@
         <v>1</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N27" s="32" t="s">
         <v>22</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P27" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q27" s="10" t="s">
         <v>23</v>
@@ -5795,9 +5827,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="8">
         <v>0</v>
@@ -5833,7 +5865,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N28" s="32" t="s">
         <v>22</v>
@@ -5852,6 +5884,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M13:M20">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5860,21 +5895,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100642169E4106A8F47AE930E47A554F108" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d50252937a7f2e196425f0325211b942">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edbcc27db5b7c97cc0de701a4705ae6f">
     <xsd:element name="properties">
@@ -5988,16 +6008,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C9F5D58-F0B6-4055-A760-0A329106689F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF32969-1B70-433C-9090-E0745F49E89E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -6012,16 +6048,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF32969-1B70-433C-9090-E0745F49E89E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C9F5D58-F0B6-4055-A760-0A329106689F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
-Integrated mem1, mem2 & changes to SP & PC
</commit_message>
<xml_diff>
--- a/Instruction bit details.xlsx
+++ b/Instruction bit details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h4z3m\Desktop\Files\College\3rd\2nd Semester\CMPN301\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06AE490-0F6C-4FBD-B4CB-62F748D97F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D16B8FC-7B2B-4259-9B8A-7FFC57C99F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="1" xr2:uid="{6DA1F6BA-0999-4314-B85B-1DD813E74D7B}"/>
+    <workbookView minimized="1" xWindow="885" yWindow="975" windowWidth="21600" windowHeight="11415" xr2:uid="{6DA1F6BA-0999-4314-B85B-1DD813E74D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -841,21 +841,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <font>
         <b val="0"/>
@@ -1555,6 +1541,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2185,11 +2178,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF38761D"/>
-      </font>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="medium">
           <color rgb="FFCCCCCC"/>
@@ -2257,6 +2245,13 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2271,57 +2266,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}" name="Table1" displayName="Table1" ref="B1:S28" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}" name="Table1" displayName="Table1" ref="B1:S28" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B1:S28" xr:uid="{279F4234-5892-4B08-BDD0-D0B119870D6F}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{8D4E3407-FC44-47DE-B88E-5309AD11F2D5}" name="Instruction" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{25C21E2B-6DEE-4078-B4A9-EA2552352DD6}" name="Mem-read" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{C5397294-29B8-4F09-9F40-E9166D94F2FE}" name="Mem-write" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{FECC954A-7C1B-40D2-86A2-FD9B4A391E20}" name="ALU src" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{23D8C483-4386-4311-BB2B-EEE7E1B86230}" name="ALU op" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{06ADF1F3-3ED4-4830-AEBB-7387DC1D335D}" name="Mem-to-reg" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{6D259160-FBA0-4881-8B80-2A2B2619FD03}" name="Branch" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{0FB6092E-1557-4466-BD9B-B56A99A8E22D}" name="Jump" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{35C25808-AE3A-4B3F-99C7-79DDCCDF49D7}" name="RegDst" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{854CF863-3B0A-454A-8E03-87707C60D946}" name="RegWrite" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{D335D4AE-F1D6-4066-A7B1-CBD1203DC43A}" name="Port EN" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{C2F17218-CFFA-4D13-AE38-39C5A8EF6E7F}" name="FlagEN" dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{D4D559F1-71F0-460D-BBFF-425684E0F856}" name="Column2" dataDxfId="30"/>
-    <tableColumn id="14" xr3:uid="{8F9EB460-835A-4CD7-AE5D-948217152F0C}" name="OpCode[5:4]" dataDxfId="29"/>
-    <tableColumn id="15" xr3:uid="{CE15952D-D927-4D54-BC82-6955E131E454}" name="OpCode[3]" dataDxfId="28"/>
-    <tableColumn id="16" xr3:uid="{9CF82271-0E8F-4CD8-9691-5677AACE840C}" name="OpCode[2]" dataDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{A5F2F74E-484F-4C42-83E9-34E52A647D2E}" name="OpCode[1]" dataDxfId="26"/>
-    <tableColumn id="18" xr3:uid="{44C370CE-309A-4F3E-9449-2EC3F32FA845}" name="OpCode[0]" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{8D4E3407-FC44-47DE-B88E-5309AD11F2D5}" name="Instruction" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{25C21E2B-6DEE-4078-B4A9-EA2552352DD6}" name="Mem-read" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{C5397294-29B8-4F09-9F40-E9166D94F2FE}" name="Mem-write" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{FECC954A-7C1B-40D2-86A2-FD9B4A391E20}" name="ALU src" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{23D8C483-4386-4311-BB2B-EEE7E1B86230}" name="ALU op" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{06ADF1F3-3ED4-4830-AEBB-7387DC1D335D}" name="Mem-to-reg" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{6D259160-FBA0-4881-8B80-2A2B2619FD03}" name="Branch" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{0FB6092E-1557-4466-BD9B-B56A99A8E22D}" name="Jump" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{35C25808-AE3A-4B3F-99C7-79DDCCDF49D7}" name="RegDst" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{854CF863-3B0A-454A-8E03-87707C60D946}" name="RegWrite" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{D335D4AE-F1D6-4066-A7B1-CBD1203DC43A}" name="Port EN" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{C2F17218-CFFA-4D13-AE38-39C5A8EF6E7F}" name="FlagEN" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{D4D559F1-71F0-460D-BBFF-425684E0F856}" name="Column2" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{8F9EB460-835A-4CD7-AE5D-948217152F0C}" name="OpCode[5:4]" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{CE15952D-D927-4D54-BC82-6955E131E454}" name="OpCode[3]" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{9CF82271-0E8F-4CD8-9691-5677AACE840C}" name="OpCode[2]" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{A5F2F74E-484F-4C42-83E9-34E52A647D2E}" name="OpCode[1]" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{44C370CE-309A-4F3E-9449-2EC3F32FA845}" name="OpCode[0]" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{37C617F5-F877-4DEE-8F3D-693EC682D08C}" name="Table13" displayName="Table13" ref="A1:R28" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{37C617F5-F877-4DEE-8F3D-693EC682D08C}" name="Table13" displayName="Table13" ref="A1:R28" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="A1:R28" xr:uid="{37C617F5-F877-4DEE-8F3D-693EC682D08C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R7">
     <sortCondition descending="1" ref="K1:K28"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{E706B79B-C3DE-40F8-8984-F90F324F38F1}" name="Instruction" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{E468DF59-6FA2-454C-A7C9-03CF45E90DFB}" name="Mem-read" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{F0E5CDCB-CD17-4F6F-99AE-47C914BBD130}" name="Mem-write" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{EAFC9A0C-24CC-4EB3-BAC2-0902DD99D451}" name="ALU src" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{72E04338-F7FE-487C-9B7C-A26811E62A38}" name="ALU op" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{A5657D19-E2E9-4349-B830-DEE87B2354AC}" name="Mem-to-reg" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{81E8A75B-C17A-4132-9D7E-2E6D2FFC70FA}" name="Branch" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{606669A1-E1A7-477E-9923-6F2C21718722}" name="Jump" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{0F6141CD-6F16-41E1-B2C7-0E368AA607E1}" name="RegDst" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{7CB9D208-D2DE-4200-8FF1-505E1FB4C112}" name="RegWrite" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{8DDC56CF-0E9C-4CE6-A782-0A8FC6FFFE69}" name="Port EN" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{4E4D1F5E-7525-4563-A551-437CC225A0A6}" name="FlagEN" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{D63ABDED-CA31-4388-8E46-DB793355A769}" name="Column2" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{7F48F358-6CED-4C7E-8A8E-28F0B0755D7F}" name="Column3" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{1DEF6221-63F2-447A-8A17-553930013B73}" name="Column4" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{A1FBB6C0-AE90-4897-B30C-3FB013B898E2}" name="Column5" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{218E459E-5EAC-478C-997C-AEC3C336D5A5}" name="Column6" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{4FC20EE3-62CA-4D56-BB07-A9DF668D2B4A}" name="Column7" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E706B79B-C3DE-40F8-8984-F90F324F38F1}" name="Instruction" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E468DF59-6FA2-454C-A7C9-03CF45E90DFB}" name="Mem-read" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{F0E5CDCB-CD17-4F6F-99AE-47C914BBD130}" name="Mem-write" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{EAFC9A0C-24CC-4EB3-BAC2-0902DD99D451}" name="ALU src" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{72E04338-F7FE-487C-9B7C-A26811E62A38}" name="ALU op" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{A5657D19-E2E9-4349-B830-DEE87B2354AC}" name="Mem-to-reg" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{81E8A75B-C17A-4132-9D7E-2E6D2FFC70FA}" name="Branch" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{606669A1-E1A7-477E-9923-6F2C21718722}" name="Jump" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{0F6141CD-6F16-41E1-B2C7-0E368AA607E1}" name="RegDst" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{7CB9D208-D2DE-4200-8FF1-505E1FB4C112}" name="RegWrite" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{8DDC56CF-0E9C-4CE6-A782-0A8FC6FFFE69}" name="Port EN" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{4E4D1F5E-7525-4563-A551-437CC225A0A6}" name="FlagEN" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{D63ABDED-CA31-4388-8E46-DB793355A769}" name="Column2" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{7F48F358-6CED-4C7E-8A8E-28F0B0755D7F}" name="Column3" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{1DEF6221-63F2-447A-8A17-553930013B73}" name="Column4" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{A1FBB6C0-AE90-4897-B30C-3FB013B898E2}" name="Column5" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{218E459E-5EAC-478C-997C-AEC3C336D5A5}" name="Column6" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{4FC20EE3-62CA-4D56-BB07-A9DF668D2B4A}" name="Column7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2626,30 +2621,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FB175E-1B2E-49A1-9201-CF52D899FEF0}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:I27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2708,7 +2703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2767,7 +2762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29" t="s">
         <v>25</v>
       </c>
@@ -2823,7 +2818,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29" t="s">
         <v>30</v>
       </c>
@@ -2879,7 +2874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="29" t="s">
         <v>32</v>
       </c>
@@ -2935,7 +2930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="29" t="s">
         <v>35</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
         <v>37</v>
       </c>
@@ -3047,7 +3042,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26" t="s">
         <v>42</v>
       </c>
@@ -3103,7 +3098,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="26" t="s">
         <v>45</v>
       </c>
@@ -3159,7 +3154,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
         <v>47</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
         <v>49</v>
       </c>
@@ -3271,7 +3266,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -3330,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>54</v>
       </c>
@@ -3386,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
         <v>55</v>
       </c>
@@ -3442,7 +3437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>56</v>
       </c>
@@ -3498,7 +3493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="42" t="s">
         <v>57</v>
       </c>
@@ -3554,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
         <v>58</v>
       </c>
@@ -3610,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
         <v>59</v>
       </c>
@@ -3666,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
         <v>60</v>
       </c>
@@ -3722,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -3778,7 +3773,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>63</v>
       </c>
@@ -3834,7 +3829,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -3893,7 +3888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>72</v>
       </c>
@@ -3949,7 +3944,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
         <v>75</v>
       </c>
@@ -4005,7 +4000,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
         <v>77</v>
       </c>
@@ -4061,7 +4056,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
         <v>79</v>
       </c>
@@ -4117,7 +4112,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="37" t="s">
         <v>81</v>
       </c>
@@ -4173,7 +4168,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="40"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -4203,7 +4198,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>84</v>
       </c>
@@ -4211,7 +4206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -4222,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -4233,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -4244,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -4255,7 +4250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>88</v>
       </c>
@@ -4275,7 +4270,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>90</v>
       </c>
@@ -4292,7 +4287,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="N2:N28">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4306,16 +4301,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CE8E6B-46C5-4A7D-9C9D-87C2DC308357}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" activeCellId="1" sqref="A24:XFD24 A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -4371,7 +4366,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>96</v>
       </c>
@@ -4427,7 +4422,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>32</v>
       </c>
@@ -4483,7 +4478,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>25</v>
       </c>
@@ -4539,7 +4534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>20</v>
       </c>
@@ -4595,7 +4590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>30</v>
       </c>
@@ -4651,7 +4646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>35</v>
       </c>
@@ -4707,7 +4702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>42</v>
       </c>
@@ -4763,7 +4758,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>47</v>
       </c>
@@ -4819,7 +4814,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>37</v>
       </c>
@@ -4875,7 +4870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>45</v>
       </c>
@@ -4931,7 +4926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>49</v>
       </c>
@@ -4987,7 +4982,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>58</v>
       </c>
@@ -5043,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>56</v>
       </c>
@@ -5099,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>55</v>
       </c>
@@ -5155,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>52</v>
       </c>
@@ -5211,7 +5206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>60</v>
       </c>
@@ -5267,7 +5262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>54</v>
       </c>
@@ -5323,7 +5318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>59</v>
       </c>
@@ -5379,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>57</v>
       </c>
@@ -5435,7 +5430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>72</v>
       </c>
@@ -5491,7 +5486,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>68</v>
       </c>
@@ -5547,7 +5542,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
@@ -5603,7 +5598,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>75</v>
       </c>
@@ -5659,7 +5654,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>79</v>
       </c>
@@ -5715,7 +5710,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>81</v>
       </c>
@@ -5771,7 +5766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>63</v>
       </c>
@@ -5827,7 +5822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>61</v>
       </c>
@@ -5885,7 +5880,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M13:M20">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5895,6 +5890,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100642169E4106A8F47AE930E47A554F108" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d50252937a7f2e196425f0325211b942">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edbcc27db5b7c97cc0de701a4705ae6f">
     <xsd:element name="properties">
@@ -6008,32 +6018,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF32969-1B70-433C-9090-E0745F49E89E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C9F5D58-F0B6-4055-A760-0A329106689F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -6048,15 +6042,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C9F5D58-F0B6-4055-A760-0A329106689F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF32969-1B70-433C-9090-E0745F49E89E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>